<commit_message>
exported data to excel
</commit_message>
<xml_diff>
--- a/in/germany_gridmix_for_Premise.xlsx
+++ b/in/germany_gridmix_for_Premise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\AWSI\GreenTech\de_gridmix\in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623BF510-E7E3-4749-A862-F0EFCD93AD8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568C5750-B889-4BFD-B731-78BB68EFD732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27750" yWindow="6810" windowWidth="23730" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8640" yWindow="240" windowWidth="23730" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA_SHORT" sheetId="6" r:id="rId1"/>
@@ -1315,7 +1315,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="H8" sqref="H8:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,6 +1456,10 @@
         <f>SUM(H2:H3)</f>
         <v>40.26</v>
       </c>
+      <c r="I4">
+        <f>SUM(I2:I3)</f>
+        <v>51.800000000000004</v>
+      </c>
       <c r="K4" t="s">
         <v>132</v>
       </c>
@@ -1667,8 +1671,23 @@
       <c r="F12">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="55">
+        <f>SUM(H4:H12)</f>
+        <v>77.17</v>
+      </c>
+      <c r="I14" s="55">
+        <f>SUM(I4:I11)</f>
+        <v>84.3</v>
+      </c>
+    </row>
     <row r="15" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1705,7 +1724,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L4"/>
+      <selection activeCell="D13" sqref="D13:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,6 +2075,12 @@
       </c>
       <c r="F12">
         <v>1.5</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -3212,8 +3237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265EC24C-A4A0-4918-A14A-F08809EDE057}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:M27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4373,8 +4398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543EFDDE-7E04-4A5D-9AAF-EF443BDA7987}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>